<commit_message>
agregado sprint 2 y 3 casi listo
</commit_message>
<xml_diff>
--- a/Documentacion/ChileWic Product Backlog.xlsx
+++ b/Documentacion/ChileWic Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\183934708\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\183934708\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,27 +21,11 @@
     <definedName name="YesNo">Sheet2!$A$6:$A$7</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="29">
-  <si>
-    <t>Task Name</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Story Points</t>
-  </si>
-  <si>
-    <t>Assigned to Sprint</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="36">
   <si>
     <t>Sprint Ready</t>
   </si>
@@ -52,24 +36,9 @@
     <t>Sprint 2</t>
   </si>
   <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
-    <t>Task 6</t>
-  </si>
-  <si>
     <t>Sprint 3</t>
   </si>
   <si>
-    <t>Task 7</t>
-  </si>
-  <si>
-    <t>Task 8</t>
-  </si>
-  <si>
     <t>Task 9</t>
   </si>
   <si>
@@ -113,13 +82,64 @@
   </si>
   <si>
     <t>Ver Asistentes registrados</t>
+  </si>
+  <si>
+    <t>Eliminar Registro de Asistencia</t>
+  </si>
+  <si>
+    <t>ChileWic Product Backlog</t>
+  </si>
+  <si>
+    <t>Asignar Revisadores</t>
+  </si>
+  <si>
+    <t>Sistema de Presupuestos</t>
+  </si>
+  <si>
+    <t>Creador de Programa</t>
+  </si>
+  <si>
+    <t>Registrar Propuesta a charlas</t>
+  </si>
+  <si>
+    <t>Modificar Propuesta a charlas</t>
+  </si>
+  <si>
+    <t>Ver Propuesta a charlas</t>
+  </si>
+  <si>
+    <t>Eliminar Propuesta a charlas</t>
+  </si>
+  <si>
+    <t>Seleccionar propuestas(Revisadores)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema autmático de asignacion de Revision    </t>
+  </si>
+  <si>
+    <t>Tarea</t>
+  </si>
+  <si>
+    <t>Entrega</t>
+  </si>
+  <si>
+    <t>Prioridad</t>
+  </si>
+  <si>
+    <t>Estatus</t>
+  </si>
+  <si>
+    <t>Puntos de Historia</t>
+  </si>
+  <si>
+    <t>Asignado a un Sprint</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,6 +192,13 @@
       <u/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,7 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -252,10 +279,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -596,24 +636,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB74"/>
+  <dimension ref="A1:AC79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.125" customWidth="1"/>
-    <col min="2" max="2" width="13.875" customWidth="1"/>
-    <col min="3" max="3" width="15.375" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
-    <col min="5" max="5" width="13.875" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="2" max="2" width="37.25" customWidth="1"/>
+    <col min="3" max="3" width="13.875" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
+    <col min="5" max="5" width="16.625" customWidth="1"/>
+    <col min="6" max="6" width="18.25" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -641,9 +680,9 @@
       <c r="Z1" s="5"/>
       <c r="AA1" s="5"/>
       <c r="AB1" s="5"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B2" s="5"/>
+      <c r="AC1" s="5"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -670,10 +709,12 @@
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
-    </row>
-    <row r="3" spans="1:28" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5"/>
+      <c r="AC2" s="5"/>
+    </row>
+    <row r="3" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -700,9 +741,9 @@
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
       <c r="AB3" s="5"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="AC3" s="5"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -730,9 +771,9 @@
       <c r="Z4" s="5"/>
       <c r="AA4" s="5"/>
       <c r="AB4" s="5"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="AC4" s="5"/>
+    </row>
+    <row r="5" spans="1:29" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -760,27 +801,30 @@
       <c r="Z5" s="5"/>
       <c r="AA5" s="5"/>
       <c r="AB5" s="5"/>
-    </row>
-    <row r="6" spans="1:28" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="AC5" s="5"/>
+    </row>
+    <row r="6" spans="1:29" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="5"/>
+      <c r="D6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -802,28 +846,29 @@
       <c r="Z6" s="5"/>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
-    </row>
-    <row r="7" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
+      <c r="AC6" s="5"/>
+    </row>
+    <row r="7" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10">
+        <v>43601</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="3">
-        <f>SUM(E8:E12)</f>
-        <v>46</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3">
+        <f>SUM(F8:F13)</f>
+        <v>24</v>
+      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -845,27 +890,27 @@
       <c r="Z7" s="5"/>
       <c r="AA7" s="5"/>
       <c r="AB7" s="5"/>
-    </row>
-    <row r="8" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="AC7" s="5"/>
+    </row>
+    <row r="8" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="2">
-        <v>8</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -887,27 +932,27 @@
       <c r="Z8" s="5"/>
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
-    </row>
-    <row r="9" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="AC8" s="5"/>
+    </row>
+    <row r="9" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="2">
-        <v>16</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -929,27 +974,27 @@
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
-    </row>
-    <row r="10" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="AC9" s="5"/>
+    </row>
+    <row r="10" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="2">
-        <v>10</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -971,31 +1016,31 @@
       <c r="Z10" s="5"/>
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
-    </row>
-    <row r="11" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="AC10" s="5"/>
+    </row>
+    <row r="11" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="2">
-        <v>8</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="8"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
@@ -1013,31 +1058,31 @@
       <c r="Z11" s="5"/>
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
-    </row>
-    <row r="12" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="AC11" s="5"/>
+    </row>
+    <row r="12" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="2">
-        <v>4</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="K12" s="8"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
@@ -1055,28 +1100,27 @@
       <c r="Z12" s="5"/>
       <c r="AA12" s="5"/>
       <c r="AB12" s="5"/>
-    </row>
-    <row r="13" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="AC12" s="5"/>
+    </row>
+    <row r="13" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="3">
-        <f>SUM(E14:E16)</f>
-        <v>96</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="5"/>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1098,27 +1142,31 @@
       <c r="Z13" s="5"/>
       <c r="AA13" s="5"/>
       <c r="AB13" s="5"/>
-    </row>
-    <row r="14" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="2">
-        <v>32</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="5"/>
+      <c r="AC13" s="5"/>
+    </row>
+    <row r="14" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>43629</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="3">
+        <f>SUM(F15:F21)</f>
+        <v>42</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1140,27 +1188,27 @@
       <c r="Z14" s="5"/>
       <c r="AA14" s="5"/>
       <c r="AB14" s="5"/>
-    </row>
-    <row r="15" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="AC14" s="5"/>
+    </row>
+    <row r="15" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="2">
-        <v>48</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1182,27 +1230,27 @@
       <c r="Z15" s="5"/>
       <c r="AA15" s="5"/>
       <c r="AB15" s="5"/>
-    </row>
-    <row r="16" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="AC15" s="5"/>
+    </row>
+    <row r="16" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="2">
-        <v>16</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="2">
+        <v>3</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -1224,28 +1272,27 @@
       <c r="Z16" s="5"/>
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
-    </row>
-    <row r="17" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="3">
-        <f>SUM(E18:E20)</f>
-        <v>32</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="5"/>
+      <c r="AC16" s="5"/>
+    </row>
+    <row r="17" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1267,27 +1314,27 @@
       <c r="Z17" s="5"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
-    </row>
-    <row r="18" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="AC17" s="5"/>
+    </row>
+    <row r="18" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="2">
-        <v>8</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="5"/>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -1309,27 +1356,27 @@
       <c r="Z18" s="5"/>
       <c r="AA18" s="5"/>
       <c r="AB18" s="5"/>
-    </row>
-    <row r="19" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="AC18" s="5"/>
+    </row>
+    <row r="19" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="2">
-        <v>8</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="2">
+        <v>10</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -1351,27 +1398,27 @@
       <c r="Z19" s="5"/>
       <c r="AA19" s="5"/>
       <c r="AB19" s="5"/>
-    </row>
-    <row r="20" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="AC19" s="5"/>
+    </row>
+    <row r="20" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="2">
-        <v>16</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -1393,15 +1440,27 @@
       <c r="Z20" s="5"/>
       <c r="AA20" s="5"/>
       <c r="AB20" s="5"/>
-    </row>
-    <row r="21" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="AC20" s="5"/>
+    </row>
+    <row r="21" spans="1:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="14">
+        <v>15</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
@@ -1416,15 +1475,38 @@
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
-    </row>
-    <row r="22" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+    </row>
+    <row r="22" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
+        <v>43639</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="3">
+        <f>SUM(F23:F25)</f>
+        <v>32</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
@@ -1439,15 +1521,34 @@
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
-    </row>
-    <row r="23" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+    </row>
+    <row r="23" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="2">
+        <v>8</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
@@ -1462,15 +1563,34 @@
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
-    </row>
-    <row r="24" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="V23" s="5"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="5"/>
+    </row>
+    <row r="24" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="2">
+        <v>8</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
@@ -1485,15 +1605,34 @@
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
       <c r="U24" s="5"/>
-    </row>
-    <row r="25" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="5"/>
+      <c r="AC24" s="5"/>
+    </row>
+    <row r="25" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="2">
+        <v>16</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
@@ -1508,9 +1647,16 @@
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
       <c r="U25" s="5"/>
-    </row>
-    <row r="26" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="5"/>
+      <c r="AC25" s="5"/>
+    </row>
+    <row r="26" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1531,9 +1677,9 @@
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
-    </row>
-    <row r="27" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
+      <c r="V26" s="5"/>
+    </row>
+    <row r="27" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1554,9 +1700,9 @@
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
-    </row>
-    <row r="28" spans="1:28" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
+      <c r="V27" s="5"/>
+    </row>
+    <row r="28" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1577,9 +1723,9 @@
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
       <c r="U28" s="5"/>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
+      <c r="V28" s="5"/>
+    </row>
+    <row r="29" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1601,15 +1747,8 @@
       <c r="T29" s="5"/>
       <c r="U29" s="5"/>
       <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
-      <c r="AB29" s="5"/>
-    </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
+    </row>
+    <row r="30" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1631,26 +1770,19 @@
       <c r="T30" s="5"/>
       <c r="U30" s="5"/>
       <c r="V30" s="5"/>
-      <c r="W30" s="5"/>
-      <c r="X30" s="5"/>
-      <c r="Y30" s="5"/>
-      <c r="Z30" s="5"/>
-      <c r="AA30" s="5"/>
-      <c r="AB30" s="5"/>
-    </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="7"/>
+    </row>
+    <row r="31" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
@@ -1661,26 +1793,19 @@
       <c r="T31" s="5"/>
       <c r="U31" s="5"/>
       <c r="V31" s="5"/>
-      <c r="W31" s="5"/>
-      <c r="X31" s="5"/>
-      <c r="Y31" s="5"/>
-      <c r="Z31" s="5"/>
-      <c r="AA31" s="5"/>
-      <c r="AB31" s="5"/>
-    </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="7"/>
+    </row>
+    <row r="32" spans="1:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
       <c r="O32" s="5"/>
@@ -1691,26 +1816,19 @@
       <c r="T32" s="5"/>
       <c r="U32" s="5"/>
       <c r="V32" s="5"/>
-      <c r="W32" s="5"/>
-      <c r="X32" s="5"/>
-      <c r="Y32" s="5"/>
-      <c r="Z32" s="5"/>
-      <c r="AA32" s="5"/>
-      <c r="AB32" s="5"/>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="7"/>
+    </row>
+    <row r="33" spans="2:29" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
       <c r="M33" s="5"/>
       <c r="N33" s="5"/>
       <c r="O33" s="5"/>
@@ -1721,26 +1839,19 @@
       <c r="T33" s="5"/>
       <c r="U33" s="5"/>
       <c r="V33" s="5"/>
-      <c r="W33" s="5"/>
-      <c r="X33" s="5"/>
-      <c r="Y33" s="5"/>
-      <c r="Z33" s="5"/>
-      <c r="AA33" s="5"/>
-      <c r="AB33" s="5"/>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="7"/>
+    </row>
+    <row r="34" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
       <c r="M34" s="5"/>
       <c r="N34" s="5"/>
       <c r="O34" s="5"/>
@@ -1757,20 +1868,20 @@
       <c r="Z34" s="5"/>
       <c r="AA34" s="5"/>
       <c r="AB34" s="5"/>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="7"/>
+      <c r="AC34" s="5"/>
+    </row>
+    <row r="35" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
       <c r="O35" s="5"/>
@@ -1787,21 +1898,21 @@
       <c r="Z35" s="5"/>
       <c r="AA35" s="5"/>
       <c r="AB35" s="5"/>
-    </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="5"/>
+      <c r="AC35" s="5"/>
+    </row>
+    <row r="36" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="7"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
       <c r="P36" s="5"/>
@@ -1817,21 +1928,21 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="5"/>
       <c r="AB36" s="5"/>
-    </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
+      <c r="AC36" s="5"/>
+    </row>
+    <row r="37" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="7"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
@@ -1847,21 +1958,21 @@
       <c r="Z37" s="5"/>
       <c r="AA37" s="5"/>
       <c r="AB37" s="5"/>
-    </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
+      <c r="AC37" s="5"/>
+    </row>
+    <row r="38" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="7"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
@@ -1877,21 +1988,21 @@
       <c r="Z38" s="5"/>
       <c r="AA38" s="5"/>
       <c r="AB38" s="5"/>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
+      <c r="AC38" s="5"/>
+    </row>
+    <row r="39" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="7"/>
       <c r="N39" s="5"/>
       <c r="O39" s="5"/>
       <c r="P39" s="5"/>
@@ -1907,21 +2018,21 @@
       <c r="Z39" s="5"/>
       <c r="AA39" s="5"/>
       <c r="AB39" s="5"/>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
+      <c r="AC39" s="5"/>
+    </row>
+    <row r="40" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="7"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
@@ -1937,21 +2048,21 @@
       <c r="Z40" s="5"/>
       <c r="AA40" s="5"/>
       <c r="AB40" s="5"/>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
+      <c r="AC40" s="5"/>
+    </row>
+    <row r="41" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="7"/>
       <c r="N41" s="5"/>
       <c r="O41" s="5"/>
       <c r="P41" s="5"/>
@@ -1967,9 +2078,9 @@
       <c r="Z41" s="5"/>
       <c r="AA41" s="5"/>
       <c r="AB41" s="5"/>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
+      <c r="AC41" s="5"/>
+    </row>
+    <row r="42" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -1997,9 +2108,9 @@
       <c r="Z42" s="5"/>
       <c r="AA42" s="5"/>
       <c r="AB42" s="5"/>
-    </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
+      <c r="AC42" s="5"/>
+    </row>
+    <row r="43" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
@@ -2027,9 +2138,9 @@
       <c r="Z43" s="5"/>
       <c r="AA43" s="5"/>
       <c r="AB43" s="5"/>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
+      <c r="AC43" s="5"/>
+    </row>
+    <row r="44" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -2057,9 +2168,9 @@
       <c r="Z44" s="5"/>
       <c r="AA44" s="5"/>
       <c r="AB44" s="5"/>
-    </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
+      <c r="AC44" s="5"/>
+    </row>
+    <row r="45" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -2087,9 +2198,9 @@
       <c r="Z45" s="5"/>
       <c r="AA45" s="5"/>
       <c r="AB45" s="5"/>
-    </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
+      <c r="AC45" s="5"/>
+    </row>
+    <row r="46" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -2117,9 +2228,9 @@
       <c r="Z46" s="5"/>
       <c r="AA46" s="5"/>
       <c r="AB46" s="5"/>
-    </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
+      <c r="AC46" s="5"/>
+    </row>
+    <row r="47" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -2147,9 +2258,9 @@
       <c r="Z47" s="5"/>
       <c r="AA47" s="5"/>
       <c r="AB47" s="5"/>
-    </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
+      <c r="AC47" s="5"/>
+    </row>
+    <row r="48" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -2177,9 +2288,9 @@
       <c r="Z48" s="5"/>
       <c r="AA48" s="5"/>
       <c r="AB48" s="5"/>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
+      <c r="AC48" s="5"/>
+    </row>
+    <row r="49" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -2207,9 +2318,9 @@
       <c r="Z49" s="5"/>
       <c r="AA49" s="5"/>
       <c r="AB49" s="5"/>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A50" s="5"/>
+      <c r="AC49" s="5"/>
+    </row>
+    <row r="50" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -2237,9 +2348,9 @@
       <c r="Z50" s="5"/>
       <c r="AA50" s="5"/>
       <c r="AB50" s="5"/>
-    </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
+      <c r="AC50" s="5"/>
+    </row>
+    <row r="51" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -2267,9 +2378,9 @@
       <c r="Z51" s="5"/>
       <c r="AA51" s="5"/>
       <c r="AB51" s="5"/>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
+      <c r="AC51" s="5"/>
+    </row>
+    <row r="52" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -2297,9 +2408,9 @@
       <c r="Z52" s="5"/>
       <c r="AA52" s="5"/>
       <c r="AB52" s="5"/>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
+      <c r="AC52" s="5"/>
+    </row>
+    <row r="53" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -2327,9 +2438,9 @@
       <c r="Z53" s="5"/>
       <c r="AA53" s="5"/>
       <c r="AB53" s="5"/>
-    </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
+      <c r="AC53" s="5"/>
+    </row>
+    <row r="54" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -2357,9 +2468,9 @@
       <c r="Z54" s="5"/>
       <c r="AA54" s="5"/>
       <c r="AB54" s="5"/>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
+      <c r="AC54" s="5"/>
+    </row>
+    <row r="55" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -2387,9 +2498,9 @@
       <c r="Z55" s="5"/>
       <c r="AA55" s="5"/>
       <c r="AB55" s="5"/>
-    </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
+      <c r="AC55" s="5"/>
+    </row>
+    <row r="56" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -2417,9 +2528,9 @@
       <c r="Z56" s="5"/>
       <c r="AA56" s="5"/>
       <c r="AB56" s="5"/>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
+      <c r="AC56" s="5"/>
+    </row>
+    <row r="57" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -2447,9 +2558,9 @@
       <c r="Z57" s="5"/>
       <c r="AA57" s="5"/>
       <c r="AB57" s="5"/>
-    </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
+      <c r="AC57" s="5"/>
+    </row>
+    <row r="58" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
@@ -2477,9 +2588,9 @@
       <c r="Z58" s="5"/>
       <c r="AA58" s="5"/>
       <c r="AB58" s="5"/>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
+      <c r="AC58" s="5"/>
+    </row>
+    <row r="59" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -2507,9 +2618,9 @@
       <c r="Z59" s="5"/>
       <c r="AA59" s="5"/>
       <c r="AB59" s="5"/>
-    </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
+      <c r="AC59" s="5"/>
+    </row>
+    <row r="60" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -2537,9 +2648,9 @@
       <c r="Z60" s="5"/>
       <c r="AA60" s="5"/>
       <c r="AB60" s="5"/>
-    </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
+      <c r="AC60" s="5"/>
+    </row>
+    <row r="61" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -2567,9 +2678,9 @@
       <c r="Z61" s="5"/>
       <c r="AA61" s="5"/>
       <c r="AB61" s="5"/>
-    </row>
-    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
+      <c r="AC61" s="5"/>
+    </row>
+    <row r="62" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -2597,9 +2708,9 @@
       <c r="Z62" s="5"/>
       <c r="AA62" s="5"/>
       <c r="AB62" s="5"/>
-    </row>
-    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A63" s="5"/>
+      <c r="AC62" s="5"/>
+    </row>
+    <row r="63" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -2627,9 +2738,9 @@
       <c r="Z63" s="5"/>
       <c r="AA63" s="5"/>
       <c r="AB63" s="5"/>
-    </row>
-    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A64" s="5"/>
+      <c r="AC63" s="5"/>
+    </row>
+    <row r="64" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
@@ -2657,9 +2768,9 @@
       <c r="Z64" s="5"/>
       <c r="AA64" s="5"/>
       <c r="AB64" s="5"/>
-    </row>
-    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A65" s="5"/>
+      <c r="AC64" s="5"/>
+    </row>
+    <row r="65" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
@@ -2687,9 +2798,9 @@
       <c r="Z65" s="5"/>
       <c r="AA65" s="5"/>
       <c r="AB65" s="5"/>
-    </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A66" s="5"/>
+      <c r="AC65" s="5"/>
+    </row>
+    <row r="66" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -2717,9 +2828,9 @@
       <c r="Z66" s="5"/>
       <c r="AA66" s="5"/>
       <c r="AB66" s="5"/>
-    </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A67" s="5"/>
+      <c r="AC66" s="5"/>
+    </row>
+    <row r="67" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -2747,9 +2858,9 @@
       <c r="Z67" s="5"/>
       <c r="AA67" s="5"/>
       <c r="AB67" s="5"/>
-    </row>
-    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
+      <c r="AC67" s="5"/>
+    </row>
+    <row r="68" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -2777,9 +2888,9 @@
       <c r="Z68" s="5"/>
       <c r="AA68" s="5"/>
       <c r="AB68" s="5"/>
-    </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
+      <c r="AC68" s="5"/>
+    </row>
+    <row r="69" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -2807,9 +2918,9 @@
       <c r="Z69" s="5"/>
       <c r="AA69" s="5"/>
       <c r="AB69" s="5"/>
-    </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
+      <c r="AC69" s="5"/>
+    </row>
+    <row r="70" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
@@ -2837,9 +2948,9 @@
       <c r="Z70" s="5"/>
       <c r="AA70" s="5"/>
       <c r="AB70" s="5"/>
-    </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
+      <c r="AC70" s="5"/>
+    </row>
+    <row r="71" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
@@ -2867,9 +2978,9 @@
       <c r="Z71" s="5"/>
       <c r="AA71" s="5"/>
       <c r="AB71" s="5"/>
-    </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
+      <c r="AC71" s="5"/>
+    </row>
+    <row r="72" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
@@ -2897,9 +3008,9 @@
       <c r="Z72" s="5"/>
       <c r="AA72" s="5"/>
       <c r="AB72" s="5"/>
-    </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A73" s="5"/>
+      <c r="AC72" s="5"/>
+    </row>
+    <row r="73" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
@@ -2927,9 +3038,9 @@
       <c r="Z73" s="5"/>
       <c r="AA73" s="5"/>
       <c r="AB73" s="5"/>
-    </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A74" s="5"/>
+      <c r="AC73" s="5"/>
+    </row>
+    <row r="74" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
@@ -2957,19 +3068,170 @@
       <c r="Z74" s="5"/>
       <c r="AA74" s="5"/>
       <c r="AB74" s="5"/>
+      <c r="AC74" s="5"/>
+    </row>
+    <row r="75" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
+      <c r="O75" s="5"/>
+      <c r="P75" s="5"/>
+      <c r="Q75" s="5"/>
+      <c r="R75" s="5"/>
+      <c r="S75" s="5"/>
+      <c r="T75" s="5"/>
+      <c r="U75" s="5"/>
+      <c r="V75" s="5"/>
+      <c r="W75" s="5"/>
+      <c r="X75" s="5"/>
+      <c r="Y75" s="5"/>
+      <c r="Z75" s="5"/>
+      <c r="AA75" s="5"/>
+      <c r="AB75" s="5"/>
+      <c r="AC75" s="5"/>
+    </row>
+    <row r="76" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+      <c r="O76" s="5"/>
+      <c r="P76" s="5"/>
+      <c r="Q76" s="5"/>
+      <c r="R76" s="5"/>
+      <c r="S76" s="5"/>
+      <c r="T76" s="5"/>
+      <c r="U76" s="5"/>
+      <c r="V76" s="5"/>
+      <c r="W76" s="5"/>
+      <c r="X76" s="5"/>
+      <c r="Y76" s="5"/>
+      <c r="Z76" s="5"/>
+      <c r="AA76" s="5"/>
+      <c r="AB76" s="5"/>
+      <c r="AC76" s="5"/>
+    </row>
+    <row r="77" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
+      <c r="G77" s="5"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5"/>
+      <c r="K77" s="5"/>
+      <c r="L77" s="5"/>
+      <c r="M77" s="5"/>
+      <c r="N77" s="5"/>
+      <c r="O77" s="5"/>
+      <c r="P77" s="5"/>
+      <c r="Q77" s="5"/>
+      <c r="R77" s="5"/>
+      <c r="S77" s="5"/>
+      <c r="T77" s="5"/>
+      <c r="U77" s="5"/>
+      <c r="V77" s="5"/>
+      <c r="W77" s="5"/>
+      <c r="X77" s="5"/>
+      <c r="Y77" s="5"/>
+      <c r="Z77" s="5"/>
+      <c r="AA77" s="5"/>
+      <c r="AB77" s="5"/>
+      <c r="AC77" s="5"/>
+    </row>
+    <row r="78" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="5"/>
+      <c r="M78" s="5"/>
+      <c r="N78" s="5"/>
+      <c r="O78" s="5"/>
+      <c r="P78" s="5"/>
+      <c r="Q78" s="5"/>
+      <c r="R78" s="5"/>
+      <c r="S78" s="5"/>
+      <c r="T78" s="5"/>
+      <c r="U78" s="5"/>
+      <c r="V78" s="5"/>
+      <c r="W78" s="5"/>
+      <c r="X78" s="5"/>
+      <c r="Y78" s="5"/>
+      <c r="Z78" s="5"/>
+      <c r="AA78" s="5"/>
+      <c r="AB78" s="5"/>
+      <c r="AC78" s="5"/>
+    </row>
+    <row r="79" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+      <c r="L79" s="5"/>
+      <c r="M79" s="5"/>
+      <c r="N79" s="5"/>
+      <c r="O79" s="5"/>
+      <c r="P79" s="5"/>
+      <c r="Q79" s="5"/>
+      <c r="R79" s="5"/>
+      <c r="S79" s="5"/>
+      <c r="T79" s="5"/>
+      <c r="U79" s="5"/>
+      <c r="V79" s="5"/>
+      <c r="W79" s="5"/>
+      <c r="X79" s="5"/>
+      <c r="Y79" s="5"/>
+      <c r="Z79" s="5"/>
+      <c r="AA79" s="5"/>
+      <c r="AB79" s="5"/>
+      <c r="AC79" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A31:K36"/>
+    <mergeCell ref="B36:L41"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7:F20 B7:B20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G7:G25 C7:C25">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D25">
       <formula1>Priority</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E25">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
@@ -2990,37 +3252,37 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>